<commit_message>
Swapped 'Analysis Title' and 'Analysis Alias' columns values in the mockup template 'Analysis' sheet
</commit_message>
<xml_diff>
--- a/src/files/EVA_Submission_template.V1.1.0_mockup.xlsx
+++ b/src/files/EVA_Submission_template.V1.1.0_mockup.xlsx
@@ -2502,6 +2502,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2512,27 +2533,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2981,7 +2981,7 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -2993,8 +2993,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -3003,10 +3003,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="80"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
@@ -3015,8 +3015,8 @@
       <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
@@ -3037,8 +3037,8 @@
       <c r="H4" s="53"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -3059,10 +3059,10 @@
       <c r="H6" s="53"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="78"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
       <c r="E7" s="54"/>
@@ -3071,8 +3071,8 @@
       <c r="H7" s="54"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="86"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -3093,8 +3093,8 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83"/>
-      <c r="B10" s="83"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3103,10 +3103,10 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" s="29" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="83" t="s">
         <v>521</v>
       </c>
-      <c r="B11" s="87"/>
+      <c r="B11" s="83"/>
     </row>
     <row r="12" spans="1:8" s="29" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
@@ -3159,28 +3159,28 @@
     </row>
     <row r="18" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="88"/>
+      <c r="B19" s="84"/>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A20" s="84" t="s">
+      <c r="A20" s="78" t="s">
         <v>524</v>
       </c>
-      <c r="B20" s="84"/>
+      <c r="B20" s="78"/>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="84" t="s">
+      <c r="A21" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="84"/>
+      <c r="B21" s="78"/>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="85"/>
+      <c r="B22" s="79"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="63" t="s">
@@ -3247,6 +3247,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A8:B8"/>
@@ -3255,12 +3261,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6176,7 +6176,7 @@
   <dimension ref="A1:AX7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6994,8 +6994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7069,11 +7069,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>561</v>
       </c>
       <c r="C2" t="s">
         <v>562</v>
@@ -7107,11 +7107,11 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>567</v>
+      </c>
+      <c r="B3">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>567</v>
       </c>
       <c r="C3" t="s">
         <v>568</v>

</xml_diff>